<commit_message>
My edits to CR_fileInit
</commit_message>
<xml_diff>
--- a/ClueLayout.xlsx
+++ b/ClueLayout.xlsx
@@ -271,66 +271,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>25</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>38</xdr:col>
-      <xdr:colOff>266699</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>77697</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2" descr="Clue Layout"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="8610600" y="228600"/>
-          <a:ext cx="8191499" cy="6478497"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -598,8 +538,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
-      <selection activeCell="P29" sqref="P29"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1858,7 +1798,7 @@
         <v>10</v>
       </c>
       <c r="I18" s="8" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="J18" s="8" t="s">
         <v>10</v>
@@ -2002,7 +1942,7 @@
         <v>10</v>
       </c>
       <c r="I20" s="8" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="J20" s="8" t="s">
         <v>10</v>
@@ -2146,7 +2086,7 @@
         <v>10</v>
       </c>
       <c r="I22" s="15" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="J22" s="15" t="s">
         <v>10</v>
@@ -2221,6 +2161,5 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Changed walway condition to make walkway W instead of A
</commit_message>
<xml_diff>
--- a/ClueLayout.xlsx
+++ b/ClueLayout.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\CSCI306\ClueGameHAMS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\csci306\ClueGameHAMS\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -32,9 +32,6 @@
     <t>X</t>
   </si>
   <si>
-    <t>A</t>
-  </si>
-  <si>
     <t>R</t>
   </si>
   <si>
@@ -59,9 +56,6 @@
     <t>P</t>
   </si>
   <si>
-    <t>WD</t>
-  </si>
-  <si>
     <t>MD</t>
   </si>
   <si>
@@ -96,6 +90,12 @@
   </si>
   <si>
     <t>UR</t>
+  </si>
+  <si>
+    <t>O</t>
+  </si>
+  <si>
+    <t>OD</t>
   </si>
 </sst>
 </file>
@@ -538,8 +538,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I23" sqref="I23"/>
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A31" sqref="A26:A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -550,529 +550,529 @@
   <sheetData>
     <row r="1" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D1" s="10" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F1" s="10" t="s">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="G1" s="10" t="s">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="H1" s="10" t="s">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="I1" s="10" t="s">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="J1" s="10" t="s">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="K1" s="10" t="s">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="L1" s="10" t="s">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="M1" s="10" t="s">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="P1" s="10" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="Q1" s="10" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="R1" s="10" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="S1" s="10" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="T1" s="10" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="U1" s="10" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="V1" s="10" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="W1" s="11" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="X1" s="1"/>
     </row>
     <row r="2" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="H2" s="8" t="s">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="I2" s="8" t="s">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="J2" s="8" t="s">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="K2" s="8" t="s">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="L2" s="8" t="s">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="M2" s="8" t="s">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O2" s="3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="P2" s="8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="Q2" s="8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="R2" s="8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="S2" s="8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="T2" s="8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="U2" s="8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="V2" s="8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="W2" s="13" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="X2" s="1"/>
     </row>
     <row r="3" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="I3" s="8" t="s">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="J3" s="8" t="s">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="K3" s="8" t="s">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="L3" s="8" t="s">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="M3" s="8" t="s">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="N3" s="3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O3" s="3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="P3" s="8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="Q3" s="8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="R3" s="8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="S3" s="8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="T3" s="8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="U3" s="8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="V3" s="8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="W3" s="13" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="X3" s="1"/>
     </row>
     <row r="4" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="H4" s="8" t="s">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="I4" s="8" t="s">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="J4" s="8" t="s">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="K4" s="8" t="s">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="L4" s="8" t="s">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="M4" s="8" t="s">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="N4" s="3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O4" s="3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="P4" s="8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="Q4" s="8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="R4" s="8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="S4" s="8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="T4" s="8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="U4" s="8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="V4" s="8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="W4" s="13" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="X4" s="1"/>
     </row>
     <row r="5" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="H5" s="8" t="s">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="I5" s="17" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="J5" s="17" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="K5" s="17" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="L5" s="8" t="s">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="M5" s="8" t="s">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="N5" s="3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O5" s="3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="P5" s="8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="Q5" s="17" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="R5" s="17" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="S5" s="8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="T5" s="8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="U5" s="8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="V5" s="8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="W5" s="13" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="X5" s="1"/>
     </row>
     <row r="6" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K6" s="3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L6" s="3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M6" s="3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N6" s="3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O6" s="3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="P6" s="3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="Q6" s="3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="R6" s="3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="S6" s="3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="T6" s="3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="U6" s="3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="V6" s="3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="W6" s="6" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="X6" s="1"/>
     </row>
     <row r="7" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D7" s="17" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J7" s="3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K7" s="3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L7" s="3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M7" s="3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N7" s="3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O7" s="3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="P7" s="3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="Q7" s="3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="R7" s="3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="S7" s="3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="T7" s="3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="U7" s="3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="V7" s="3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="W7" s="6" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="X7" s="1"/>
     </row>
     <row r="8" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D8" s="17" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H8" s="4" t="s">
         <v>1</v>
@@ -1099,52 +1099,52 @@
         <v>1</v>
       </c>
       <c r="P8" s="3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="Q8" s="3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="R8" s="8" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="S8" s="17" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="T8" s="8" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="U8" s="8" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="V8" s="8" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="W8" s="13" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="X8" s="1"/>
     </row>
     <row r="9" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H9" s="4" t="s">
         <v>1</v>
@@ -1171,52 +1171,52 @@
         <v>1</v>
       </c>
       <c r="P9" s="3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="Q9" s="3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="R9" s="8" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="S9" s="8" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="T9" s="8" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="U9" s="8" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="V9" s="8" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="W9" s="13" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="X9" s="1"/>
     </row>
     <row r="10" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H10" s="4" t="s">
         <v>1</v>
@@ -1243,52 +1243,52 @@
         <v>1</v>
       </c>
       <c r="P10" s="3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="Q10" s="3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="R10" s="8" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="S10" s="8" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="T10" s="8" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="U10" s="8" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="V10" s="8" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="W10" s="13" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="X10" s="1"/>
     </row>
     <row r="11" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H11" s="4" t="s">
         <v>1</v>
@@ -1315,52 +1315,52 @@
         <v>1</v>
       </c>
       <c r="P11" s="3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="Q11" s="3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="R11" s="8" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="S11" s="8" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="T11" s="8" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="U11" s="8" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="V11" s="8" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="W11" s="13" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="X11" s="1"/>
     </row>
     <row r="12" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H12" s="4" t="s">
         <v>1</v>
@@ -1387,52 +1387,52 @@
         <v>1</v>
       </c>
       <c r="P12" s="3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="Q12" s="3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="R12" s="8" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="S12" s="8" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="T12" s="8" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="U12" s="8" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="V12" s="8" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="W12" s="13" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="X12" s="1"/>
     </row>
     <row r="13" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H13" s="4" t="s">
         <v>1</v>
@@ -1459,676 +1459,676 @@
         <v>1</v>
       </c>
       <c r="P13" s="3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="Q13" s="3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="R13" s="8" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="S13" s="8" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="T13" s="8" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="U13" s="8" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="V13" s="8" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="W13" s="13" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="X13" s="1"/>
     </row>
     <row r="14" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="19" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I14" s="3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J14" s="3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K14" s="3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L14" s="3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M14" s="3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N14" s="3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O14" s="3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="P14" s="3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="Q14" s="3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="R14" s="8" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="S14" s="8" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="T14" s="8" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="U14" s="8" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="V14" s="8" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="W14" s="13" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="X14" s="1"/>
     </row>
     <row r="15" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I15" s="3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J15" s="3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K15" s="3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L15" s="3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M15" s="3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N15" s="3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O15" s="3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="P15" s="3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="Q15" s="3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="R15" s="8" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="S15" s="17" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="T15" s="8" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="U15" s="8" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="V15" s="8" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="W15" s="13" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="X15" s="1"/>
     </row>
     <row r="16" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="19" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I16" s="3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J16" s="3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K16" s="3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L16" s="3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M16" s="8" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="N16" s="17" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="O16" s="3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="P16" s="3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="Q16" s="3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="R16" s="3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="S16" s="3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="T16" s="3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="U16" s="3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="V16" s="3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="W16" s="6" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="X16" s="1"/>
     </row>
     <row r="17" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D17" s="17" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G17" s="8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H17" s="8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I17" s="17" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="J17" s="8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="K17" s="8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="L17" s="3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M17" s="8" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="N17" s="17" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="O17" s="3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="P17" s="3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="Q17" s="3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="R17" s="3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="S17" s="3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="T17" s="17" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="U17" s="8" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="V17" s="8" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="W17" s="13" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="X17" s="1"/>
     </row>
     <row r="18" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G18" s="8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H18" s="8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I18" s="8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J18" s="8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="K18" s="8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="L18" s="3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M18" s="8" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="N18" s="8" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="O18" s="8" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="P18" s="8" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="Q18" s="8" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="R18" s="3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="S18" s="3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="T18" s="17" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="U18" s="8" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="V18" s="8" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="W18" s="13" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="X18" s="1"/>
     </row>
     <row r="19" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G19" s="8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H19" s="8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I19" s="8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J19" s="8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="K19" s="8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="L19" s="3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M19" s="8" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="N19" s="8" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="O19" s="8" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="P19" s="8" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="Q19" s="8" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="R19" s="3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="S19" s="3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="T19" s="8" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="U19" s="8" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="V19" s="8" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="W19" s="13" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="X19" s="1"/>
     </row>
     <row r="20" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G20" s="8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H20" s="8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I20" s="8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J20" s="8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="K20" s="8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="L20" s="3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M20" s="8" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="N20" s="8" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="O20" s="8" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="P20" s="8" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="Q20" s="8" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="R20" s="3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="S20" s="3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="T20" s="8" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="U20" s="8" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="V20" s="8" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="W20" s="13" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="X20" s="1"/>
     </row>
     <row r="21" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G21" s="8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H21" s="8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I21" s="8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J21" s="8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="K21" s="8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="L21" s="3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M21" s="8" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="N21" s="8" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="O21" s="8" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="P21" s="8" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="Q21" s="8" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="R21" s="3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="S21" s="3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="T21" s="8" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="U21" s="8" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="V21" s="8" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="W21" s="13" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="X21" s="1"/>
     </row>
     <row r="22" spans="1:24" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="14" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B22" s="15" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C22" s="15" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D22" s="15" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E22" s="7" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F22" s="7" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G22" s="15" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H22" s="15" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I22" s="15" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J22" s="15" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="K22" s="18" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="L22" s="7" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M22" s="18" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="N22" s="15" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="O22" s="15" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="P22" s="15" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="Q22" s="15" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="R22" s="7" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="S22" s="7" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="T22" s="15" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="U22" s="15" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="V22" s="15" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="W22" s="16" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="X22" s="1"/>
     </row>

</xml_diff>